<commit_message>
Have non-corner cases of choose_players working
</commit_message>
<xml_diff>
--- a/btsAccounts.xlsx
+++ b/btsAccounts.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -71,6 +71,15 @@
   </si>
   <si>
     <t>faiyamR003@gmail.com</t>
+  </si>
+  <si>
+    <t>singleBot(LOCKED)</t>
+  </si>
+  <si>
+    <t>faiyamR004@gmail.com</t>
+  </si>
+  <si>
+    <t>beatthestreak4</t>
   </si>
 </sst>
 </file>
@@ -474,15 +483,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="A1:E4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
@@ -525,7 +534,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>15</v>
@@ -555,6 +564,23 @@
       </c>
       <c r="E4" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -562,6 +588,7 @@
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Added first production level email to btsAccounts
</commit_message>
<xml_diff>
--- a/btsAccounts.xlsx
+++ b/btsAccounts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16100" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="12220" yWindow="0" windowWidth="16100" windowHeight="15560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>ID</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>For receiving error logs</t>
+  </si>
+  <si>
+    <t>faiyam.daft.54@gmail.com</t>
+  </si>
+  <si>
+    <t>sdFgsdfg892m45</t>
   </si>
 </sst>
 </file>
@@ -500,7 +506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -617,10 +623,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -649,7 +655,24 @@
         <v>8</v>
       </c>
     </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
moving from faiyam to dmoneys computer
</commit_message>
<xml_diff>
--- a/btsAccounts.xlsx
+++ b/btsAccounts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12220" yWindow="0" windowWidth="16100" windowHeight="15560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -99,6 +99,15 @@
   </si>
   <si>
     <t>sdFgsdfg892m45</t>
+  </si>
+  <si>
+    <t>water_earth_402@yahoo.com</t>
+  </si>
+  <si>
+    <t>helloGoe234</t>
+  </si>
+  <si>
+    <t>daft_williams_405@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -154,7 +163,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -162,16 +171,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="10">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
@@ -507,7 +522,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -623,16 +638,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
@@ -669,9 +684,54 @@
         <v>25</v>
       </c>
     </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
accounts.py passed its first end to end test
</commit_message>
<xml_diff>
--- a/btsAccounts.xlsx
+++ b/btsAccounts.xlsx
@@ -1,83 +1,149 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <s:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <s:bookViews>
-    <s:workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Production" sheetId="1" r:id="rId1"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="500" activeTab="1"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Test" sheetId="1" r:id="rId1"/>
+    <sheet name="Production" sheetId="2" r:id="rId2"/>
+    <sheet name="Other" sheetId="3" r:id="rId3"/>
+  </sheets>
+  <calcPr calcId="140000" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+  <si>
+    <t>ID</t>
+  </si>
   <si>
     <t>Email</t>
   </si>
   <si>
+    <t>beatthestreak1</t>
+  </si>
+  <si>
+    <t>beatthestreak2</t>
+  </si>
+  <si>
+    <t>beatthestreak3</t>
+  </si>
+  <si>
+    <t>emptyBot</t>
+  </si>
+  <si>
+    <t>singleBot</t>
+  </si>
+  <si>
+    <t>doubleBot</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>no selections</t>
+  </si>
+  <si>
+    <t>one selection</t>
+  </si>
+  <si>
+    <t>double down selection</t>
+  </si>
+  <si>
     <t>EmailPassword</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>MLBPassword</t>
   </si>
   <si>
-    <t>beatthestreak1</t>
-  </si>
-  <si>
-    <t>beatthestreak3</t>
+    <t>faiyamR001@gmail.com</t>
+  </si>
+  <si>
+    <t>faiyamR002@gmail.com</t>
+  </si>
+  <si>
+    <t>faiyamR003@gmail.com</t>
+  </si>
+  <si>
+    <t>singleBot(LOCKED)</t>
+  </si>
+  <si>
+    <t>faiyamR004@gmail.com</t>
+  </si>
+  <si>
+    <t>beatthestreak4</t>
+  </si>
+  <si>
+    <t>faiyamerror@gmail.com</t>
+  </si>
+  <si>
+    <t>beatthestreakAdmin</t>
+  </si>
+  <si>
+    <t>N/a</t>
+  </si>
+  <si>
+    <t>For receiving error logs</t>
+  </si>
+  <si>
+    <t>faiyam.daft.54@gmail.com</t>
+  </si>
+  <si>
+    <t>sdFgsdfg892m45</t>
+  </si>
+  <si>
+    <t>water_earth_402@yahoo.com</t>
+  </si>
+  <si>
+    <t>helloGoe234</t>
   </si>
   <si>
     <t>daft_williams_405@yahoo.com</t>
-  </si>
-  <si>
-    <t>earth.water.1824@NETORG112903.onmicrosoft.com</t>
-  </si>
-  <si>
-    <t>faiyam.daft.54@gmail.com</t>
-  </si>
-  <si>
-    <t>faiyamR003@gmail.com</t>
-  </si>
-  <si>
-    <t>helloGoe234</t>
-  </si>
-  <si>
-    <t>n/a</t>
-  </si>
-  <si>
-    <t>sdFgsdfg892m45</t>
-  </si>
-  <si>
-    <t>water_earth_402@yahoo.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -88,7 +154,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -96,36 +162,38 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+  <cellStyleXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+  <cellStyles count="10">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -134,10 +202,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -204,6 +272,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -238,6 +307,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -272,20 +342,16 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -293,7 +359,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -302,13 +368,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -318,7 +384,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -327,7 +393,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -336,7 +402,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -346,12 +412,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -382,7 +448,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -401,120 +467,338 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
-  </sheetPr>
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.10"/>
-    <col min="2" max="2" width="9.10"/>
-    <col min="3" max="3" width="9.10"/>
-    <col min="4" max="4" width="9.10"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c s="1" r="A1" t="s">
+    <row r="1" spans="1:5" ht="25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c s="1" r="B1" t="s">
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c s="1" r="C1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c s="1" r="D1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="n">
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B3" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="n">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Account creation is now working from end to end
</commit_message>
<xml_diff>
--- a/btsAccounts.xlsx
+++ b/btsAccounts.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24526"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620"/>
   </bookViews>
   <sheets>
-    <sheet name="Test" sheetId="1" r:id="rId1"/>
-    <sheet name="Production" sheetId="2" r:id="rId2"/>
+    <sheet name="Production" sheetId="1" r:id="rId1"/>
+    <sheet name="Test" sheetId="2" r:id="rId2"/>
     <sheet name="Other" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,12 +21,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>EmailPassword</t>
+  </si>
+  <si>
+    <t>For receiving error logs</t>
+  </si>
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>Email</t>
+    <t>MLBPassword</t>
+  </si>
+  <si>
+    <t>N/a</t>
+  </si>
+  <si>
+    <t>Notes:</t>
   </si>
   <si>
     <t>beatthestreak1</t>
@@ -38,76 +53,55 @@
     <t>beatthestreak3</t>
   </si>
   <si>
+    <t>beatthestreak4</t>
+  </si>
+  <si>
+    <t>beatthestreakAdmin</t>
+  </si>
+  <si>
+    <t>double down selection</t>
+  </si>
+  <si>
+    <t>doubleBot</t>
+  </si>
+  <si>
     <t>emptyBot</t>
   </si>
   <si>
+    <t>faiyamR001@gmail.com</t>
+  </si>
+  <si>
+    <t>faiyamR002@gmail.com</t>
+  </si>
+  <si>
+    <t>faiyamR003@gmail.com</t>
+  </si>
+  <si>
+    <t>faiyamR004@gmail.com</t>
+  </si>
+  <si>
+    <t>faiyamerror@gmail.com</t>
+  </si>
+  <si>
+    <t>fossil.williams.1140@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>no selections</t>
+  </si>
+  <si>
+    <t>one selection</t>
+  </si>
+  <si>
     <t>singleBot</t>
   </si>
   <si>
-    <t>doubleBot</t>
-  </si>
-  <si>
-    <t>Notes:</t>
-  </si>
-  <si>
-    <t>no selections</t>
-  </si>
-  <si>
-    <t>one selection</t>
-  </si>
-  <si>
-    <t>double down selection</t>
-  </si>
-  <si>
-    <t>EmailPassword</t>
-  </si>
-  <si>
-    <t>MLBPassword</t>
-  </si>
-  <si>
-    <t>faiyamR001@gmail.com</t>
-  </si>
-  <si>
-    <t>faiyamR002@gmail.com</t>
-  </si>
-  <si>
-    <t>faiyamR003@gmail.com</t>
-  </si>
-  <si>
     <t>singleBot(LOCKED)</t>
   </si>
   <si>
-    <t>faiyamR004@gmail.com</t>
-  </si>
-  <si>
-    <t>beatthestreak4</t>
-  </si>
-  <si>
-    <t>faiyamerror@gmail.com</t>
-  </si>
-  <si>
-    <t>beatthestreakAdmin</t>
-  </si>
-  <si>
-    <t>N/a</t>
-  </si>
-  <si>
-    <t>For receiving error logs</t>
-  </si>
-  <si>
-    <t>faiyam.daft.54@gmail.com</t>
-  </si>
-  <si>
-    <t>sdFgsdfg892m45</t>
-  </si>
-  <si>
-    <t>water_earth_402@yahoo.com</t>
-  </si>
-  <si>
-    <t>helloGoe234</t>
-  </si>
-  <si>
-    <t>daft_williams_405@yahoo.com</t>
+    <t>faiyam@faiyamrahman.com</t>
   </si>
 </sst>
 </file>
@@ -116,7 +110,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -124,14 +118,14 @@
     </font>
     <font>
       <b/>
-      <sz val="20"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -139,7 +133,7 @@
     </font>
     <font>
       <u/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -154,7 +148,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -162,38 +156,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -272,7 +269,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -307,7 +303,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -342,16 +337,20 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -473,158 +472,72 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -640,99 +553,96 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
         <v>24</v>
       </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>16</v>
+      <c r="B5" t="s">
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B5" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B3" r:id="rId4"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -746,54 +656,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="A1:E2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="B2" s="2" t="s">
-        <v>20</v>
+      <c r="B2" t="s">
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Removed email creation from the account creatrion process. We'll just retroactively make the emaisl we need for the accounts that get high streaks. Moved bot webdriver to chrome, because its stabler
</commit_message>
<xml_diff>
--- a/btsAccounts.xlsx
+++ b/btsAccounts.xlsx
@@ -1,27 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24526"/>
-  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Production" sheetId="1" r:id="rId1"/>
-    <sheet name="Test" sheetId="2" r:id="rId2"/>
-    <sheet name="Other" sheetId="3" r:id="rId3"/>
-  </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
-</workbook>
+<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <s:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <s:bookViews>
+    <s:workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+  </s:bookViews>
+  <s:sheets>
+    <s:sheet name="Production" sheetId="1" r:id="rId1"/>
+    <s:sheet name="Test" sheetId="2" r:id="rId2"/>
+    <s:sheet name="Other" sheetId="3" r:id="rId3"/>
+  </s:sheets>
+  <s:definedNames/>
+  <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
+</s:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
   <si>
     <t>Email</t>
   </si>
@@ -59,15 +55,36 @@
     <t>beatthestreakAdmin</t>
   </si>
   <si>
+    <t>bts.metro.1385@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>daft.earth.1870@faiyamrahman.com</t>
+  </si>
+  <si>
     <t>double down selection</t>
   </si>
   <si>
     <t>doubleBot</t>
   </si>
   <si>
+    <t>earth.williams.1801@faiyamrahman.com</t>
+  </si>
+  <si>
     <t>emptyBot</t>
   </si>
   <si>
+    <t>faiyam.daft.1515@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>faiyam.earth.1200@NETORG112903.onmicrosoft.com</t>
+  </si>
+  <si>
+    <t>faiyam.water.1983@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>faiyam@faiyamrahman.com</t>
+  </si>
+  <si>
     <t>faiyamR001@gmail.com</t>
   </si>
   <si>
@@ -86,6 +103,15 @@
     <t>fossil.williams.1140@faiyamrahman.com</t>
   </si>
   <si>
+    <t>fossil.williams.764@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>grassfed.bts.398@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>metro.grassfed.828@faiyamrahman.com</t>
+  </si>
+  <si>
     <t>n/a</t>
   </si>
   <si>
@@ -95,20 +121,39 @@
     <t>one selection</t>
   </si>
   <si>
+    <t>rahman.bts.286@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>rahman.williams.325@faiyamrahman.com</t>
+  </si>
+  <si>
     <t>singleBot</t>
   </si>
   <si>
     <t>singleBot(LOCKED)</t>
   </si>
   <si>
-    <t>faiyam@faiyamrahman.com</t>
+    <t>water.metro.1851@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>water.rahman.227@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>williams.daft.1299@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>williams.daft.1832@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>williams.daft.741@faiyamrahman.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,27 +162,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b/>
     </font>
   </fonts>
   <fills count="2">
@@ -172,25 +201,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="1">
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -199,10 +223,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -358,7 +382,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -367,13 +391,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -383,7 +407,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -392,7 +416,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -401,7 +425,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -411,12 +435,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -447,7 +471,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -466,7 +490,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -478,108 +502,337 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
+  </sheetPr>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.10"/>
+    <col min="2" max="2" width="9.10"/>
+    <col min="3" max="3" width="9.10"/>
+    <col min="4" max="4" width="9.10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c s="1" r="A1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c s="1" r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c s="1" r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c s="1" r="D1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2">
+      <c r="A2" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>26</v>
+      <c r="B2" t="s">
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3">
+      <c r="A3" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
+  </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1" activeCell="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.10"/>
+    <col min="2" max="2" width="9.10"/>
+    <col min="3" max="3" width="9.10"/>
+    <col min="4" max="4" width="9.10"/>
+    <col min="5" max="5" width="9.10"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c s="1" r="A1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c s="1" r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c s="1" r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c s="1" r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c s="1" r="E1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -588,15 +841,15 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -605,15 +858,15 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -622,15 +875,15 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -639,47 +892,53 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
+  </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1" activeCell="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.10"/>
+    <col min="2" max="2" width="9.10"/>
+    <col min="3" max="3" width="9.10"/>
+    <col min="4" max="4" width="9.10"/>
+    <col min="5" max="5" width="9.10"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c s="1" r="A1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c s="1" r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c s="1" r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c s="1" r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c s="1" r="E1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="B2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -692,11 +951,5 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
made a test btsAccountsfile and edited filepath to return its path
</commit_message>
<xml_diff>
--- a/btsAccounts.xlsx
+++ b/btsAccounts.xlsx
@@ -4,12 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24526"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620"/>
+    <workbookView xWindow="-380" yWindow="0" windowWidth="13020" windowHeight="15620"/>
   </bookViews>
   <sheets>
     <sheet name="Production" sheetId="1" r:id="rId1"/>
-    <sheet name="Test" sheetId="2" r:id="rId2"/>
-    <sheet name="Other" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="106">
   <si>
     <t>Email</t>
   </si>
@@ -29,36 +27,15 @@
     <t>EmailPassword</t>
   </si>
   <si>
-    <t>For receiving error logs</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
     <t>MLBPassword</t>
   </si>
   <si>
-    <t>N/a</t>
-  </si>
-  <si>
-    <t>Notes:</t>
-  </si>
-  <si>
     <t>beatthestreak1</t>
   </si>
   <si>
-    <t>beatthestreak2</t>
-  </si>
-  <si>
-    <t>beatthestreak3</t>
-  </si>
-  <si>
-    <t>beatthestreak4</t>
-  </si>
-  <si>
-    <t>beatthestreakAdmin</t>
-  </si>
-  <si>
     <t>bts.bts.1358@faiyamrahman.com</t>
   </si>
   <si>
@@ -119,12 +96,6 @@
     <t>daft.williams.762@faiyamrahman.com</t>
   </si>
   <si>
-    <t>double down selection</t>
-  </si>
-  <si>
-    <t>doubleBot</t>
-  </si>
-  <si>
     <t>earth.bts.1845@faiyamrahman.com</t>
   </si>
   <si>
@@ -152,9 +123,6 @@
     <t>earth.williams.1801@faiyamrahman.com</t>
   </si>
   <si>
-    <t>emptyBot</t>
-  </si>
-  <si>
     <t>faiyam.bts.1554@faiyamrahman.com</t>
   </si>
   <si>
@@ -188,21 +156,6 @@
     <t>faiyam@faiyamrahman.com</t>
   </si>
   <si>
-    <t>faiyamR001@gmail.com</t>
-  </si>
-  <si>
-    <t>faiyamR002@gmail.com</t>
-  </si>
-  <si>
-    <t>faiyamR003@gmail.com</t>
-  </si>
-  <si>
-    <t>faiyamR004@gmail.com</t>
-  </si>
-  <si>
-    <t>faiyamerror@gmail.com</t>
-  </si>
-  <si>
     <t>fossil.bts.1000@faiyamrahman.com</t>
   </si>
   <si>
@@ -305,12 +258,6 @@
     <t>n/a</t>
   </si>
   <si>
-    <t>no selections</t>
-  </si>
-  <si>
-    <t>one selection</t>
-  </si>
-  <si>
     <t>rahman.bts.286@faiyamrahman.com</t>
   </si>
   <si>
@@ -339,12 +286,6 @@
   </si>
   <si>
     <t>rahman.williams.945@faiyamrahman.com</t>
-  </si>
-  <si>
-    <t>singleBot</t>
-  </si>
-  <si>
-    <t>singleBot(LOCKED)</t>
   </si>
   <si>
     <t>water.bts.1186@faiyamrahman.com</t>
@@ -768,7 +709,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -777,7 +718,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -785,13 +726,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -799,13 +740,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -813,13 +754,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -827,13 +768,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -841,13 +782,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -855,13 +796,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -869,13 +810,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="C8" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -883,13 +824,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -897,13 +838,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -911,13 +852,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="C11" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -925,13 +866,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -939,13 +880,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -953,13 +894,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -967,13 +908,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="C15" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -981,13 +922,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -995,13 +936,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="C17" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1009,13 +950,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D18" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1023,13 +964,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="C19" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1037,13 +978,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1051,13 +992,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1065,13 +1006,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D22" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1079,13 +1020,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D23" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1093,13 +1034,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="C24" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D24" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1107,13 +1048,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="C25" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D25" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1121,13 +1062,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="C26" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D26" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1135,13 +1076,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="C27" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1149,13 +1090,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C28" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D28" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1163,13 +1104,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="C29" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D29" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1177,13 +1118,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C30" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1191,13 +1132,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D31" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1205,13 +1146,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="C32" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D32" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1219,13 +1160,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="C33" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D33" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1233,13 +1174,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="C34" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D34" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1247,13 +1188,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="C35" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D35" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1261,13 +1202,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="C36" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D36" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1275,13 +1216,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="C37" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D37" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1289,13 +1230,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C38" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D38" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1303,13 +1244,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="C39" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D39" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1317,13 +1258,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="C40" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D40" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1331,13 +1272,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="C41" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D41" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1345,13 +1286,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C42" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D42" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1359,13 +1300,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C43" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D43" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1373,13 +1314,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C44" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D44" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1387,13 +1328,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="C45" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D45" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1401,13 +1342,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="C46" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D46" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1415,13 +1356,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C47" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D47" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1429,13 +1370,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D48" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1443,13 +1384,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C49" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D49" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1457,13 +1398,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C50" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D50" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1471,13 +1412,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C51" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D51" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1485,13 +1426,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C52" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D52" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1499,13 +1440,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C53" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D53" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1513,13 +1454,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C54" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D54" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1527,13 +1468,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C55" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D55" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1541,13 +1482,13 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C56" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D56" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1555,13 +1496,13 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="C57" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D57" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1569,13 +1510,13 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="C58" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D58" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1583,13 +1524,13 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C59" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D59" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1597,13 +1538,13 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C60" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D60" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1611,13 +1552,13 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="C61" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D61" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1625,13 +1566,13 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C62" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D62" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1639,13 +1580,13 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C63" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D63" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1653,13 +1594,13 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="C64" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D64" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1667,13 +1608,13 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="C65" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D65" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1681,13 +1622,13 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="C66" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D66" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1695,13 +1636,13 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C67" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D67" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1709,13 +1650,13 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C68" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D68" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1723,13 +1664,13 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C69" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D69" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1737,13 +1678,13 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C70" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D70" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1751,13 +1692,13 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="C71" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D71" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1765,13 +1706,13 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="C72" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D72" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1779,13 +1720,13 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C73" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D73" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1793,13 +1734,13 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C74" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D74" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1807,13 +1748,13 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C75" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D75" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1821,13 +1762,13 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="C76" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D76" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1835,13 +1776,13 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="C77" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D77" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1849,13 +1790,13 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="C78" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D78" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1863,13 +1804,13 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C79" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D79" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1877,13 +1818,13 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="C80" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D80" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1891,13 +1832,13 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="C81" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D81" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1905,13 +1846,13 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C82" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D82" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1919,13 +1860,13 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C83" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D83" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1933,13 +1874,13 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="C84" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D84" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -1947,13 +1888,13 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="C85" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D85" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1961,13 +1902,13 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="C86" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D86" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -1975,13 +1916,13 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C87" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D87" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -1989,13 +1930,13 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C88" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D88" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -2003,13 +1944,13 @@
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="C89" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D89" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -2017,13 +1958,13 @@
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C90" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D90" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -2031,13 +1972,13 @@
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="C91" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D91" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2045,13 +1986,13 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="C92" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D92" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -2059,13 +2000,13 @@
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="C93" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D93" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -2073,13 +2014,13 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C94" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D94" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2087,13 +2028,13 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="C95" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D95" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2101,13 +2042,13 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C96" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D96" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2115,13 +2056,13 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="C97" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D97" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2129,13 +2070,13 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C98" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D98" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2143,13 +2084,13 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C99" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D99" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -2157,13 +2098,13 @@
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="C100" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D100" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -2171,165 +2112,13 @@
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="C101" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D101" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="B2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reduced the test accounts excel file down to 2, for faster testing
</commit_message>
<xml_diff>
--- a/btsAccounts.xlsx
+++ b/btsAccounts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24526"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-380" yWindow="0" windowWidth="13020" windowHeight="15620"/>
+    <workbookView xWindow="160" yWindow="0" windowWidth="13720" windowHeight="15620"/>
   </bookViews>
   <sheets>
     <sheet name="Production" sheetId="1" r:id="rId1"/>
@@ -343,7 +343,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,6 +357,22 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -391,8 +407,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -400,7 +418,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -696,7 +716,7 @@
   <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2123,6 +2143,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
create 50 more accounts
</commit_message>
<xml_diff>
--- a/btsAccounts.xlsx
+++ b/btsAccounts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24526"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="0" windowWidth="13720" windowHeight="15620"/>
+    <workbookView xWindow="4580" yWindow="240" windowWidth="25280" windowHeight="15380"/>
   </bookViews>
   <sheets>
     <sheet name="Production" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="156">
   <si>
     <t>Email</t>
   </si>
@@ -337,6 +337,156 @@
   </si>
   <si>
     <t>williams.water.1647@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>fossil.daft.1579@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>fossil.earth.1755@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>faiyam.williams.524@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>grassfed.faiyam.592@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>rahman.grassfed.1726@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>williams.bts.1129@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>williams.faiyam.109@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>faiyam.bts.822@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>bts.rahman.1030@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>williams.rahman.1847@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>grassfed.bts.805@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>rahman.rahman.602@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>earth.bts.1735@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>williams.faiyam.12@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>bts.grassfed.1860@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>fossil.water.365@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>bts.daft.132@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>rahman.williams.242@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>faiyam.williams.694@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>fossil.grassfed.1308@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>bts.rahman.1114@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>bts.williams.1249@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>williams.earth.1048@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>faiyam.faiyam.1624@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>faiyam.fossil.153@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>faiyam.earth.739@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>fossil.bts.428@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>earth.rahman.1730@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>rahman.earth.923@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>williams.metro.831@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>rahman.bts.894@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>water.grassfed.484@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>metro.bts.15@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>earth.faiyam.1142@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>grassfed.fossil.708@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>grassfed.metro.1425@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>bts.grassfed.1311@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>williams.grassfed.1983@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>earth.water.785@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>bts.daft.516@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>daft.williams.1509@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>rahman.williams.919@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>rahman.daft.1669@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>metro.williams.1661@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>rahman.williams.697@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>rahman.daft.760@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>metro.faiyam.597@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>fossil.fossil.1380@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>metro.earth.1457@faiyamrahman.com</t>
+  </si>
+  <si>
+    <t>williams.daft.1236@faiyamrahman.com</t>
   </si>
 </sst>
 </file>
@@ -713,15 +863,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="B155" sqref="B155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" customWidth="1"/>
     <col min="2" max="2" width="41.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
@@ -2138,6 +2288,706 @@
         <v>78</v>
       </c>
       <c r="D101" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102">
+        <v>100</v>
+      </c>
+      <c r="B102" t="s">
+        <v>155</v>
+      </c>
+      <c r="C102" t="s">
+        <v>78</v>
+      </c>
+      <c r="D102" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103">
+        <v>101</v>
+      </c>
+      <c r="B103" t="s">
+        <v>154</v>
+      </c>
+      <c r="C103" t="s">
+        <v>78</v>
+      </c>
+      <c r="D103" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104">
+        <v>102</v>
+      </c>
+      <c r="B104" t="s">
+        <v>153</v>
+      </c>
+      <c r="C104" t="s">
+        <v>78</v>
+      </c>
+      <c r="D104" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105">
+        <v>103</v>
+      </c>
+      <c r="B105" t="s">
+        <v>152</v>
+      </c>
+      <c r="C105" t="s">
+        <v>78</v>
+      </c>
+      <c r="D105" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106">
+        <v>104</v>
+      </c>
+      <c r="B106" t="s">
+        <v>151</v>
+      </c>
+      <c r="C106" t="s">
+        <v>78</v>
+      </c>
+      <c r="D106" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107">
+        <v>105</v>
+      </c>
+      <c r="B107" t="s">
+        <v>150</v>
+      </c>
+      <c r="C107" t="s">
+        <v>78</v>
+      </c>
+      <c r="D107" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108">
+        <v>106</v>
+      </c>
+      <c r="B108" t="s">
+        <v>149</v>
+      </c>
+      <c r="C108" t="s">
+        <v>78</v>
+      </c>
+      <c r="D108" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109">
+        <v>107</v>
+      </c>
+      <c r="B109" t="s">
+        <v>148</v>
+      </c>
+      <c r="C109" t="s">
+        <v>78</v>
+      </c>
+      <c r="D109" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110">
+        <v>108</v>
+      </c>
+      <c r="B110" t="s">
+        <v>147</v>
+      </c>
+      <c r="C110" t="s">
+        <v>78</v>
+      </c>
+      <c r="D110" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111">
+        <v>109</v>
+      </c>
+      <c r="B111" t="s">
+        <v>146</v>
+      </c>
+      <c r="C111" t="s">
+        <v>78</v>
+      </c>
+      <c r="D111" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112">
+        <v>110</v>
+      </c>
+      <c r="B112" t="s">
+        <v>145</v>
+      </c>
+      <c r="C112" t="s">
+        <v>78</v>
+      </c>
+      <c r="D112" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113">
+        <v>111</v>
+      </c>
+      <c r="B113" t="s">
+        <v>144</v>
+      </c>
+      <c r="C113" t="s">
+        <v>78</v>
+      </c>
+      <c r="D113" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114">
+        <v>112</v>
+      </c>
+      <c r="B114" t="s">
+        <v>143</v>
+      </c>
+      <c r="C114" t="s">
+        <v>78</v>
+      </c>
+      <c r="D114" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115">
+        <v>113</v>
+      </c>
+      <c r="B115" t="s">
+        <v>142</v>
+      </c>
+      <c r="C115" t="s">
+        <v>78</v>
+      </c>
+      <c r="D115" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116">
+        <v>114</v>
+      </c>
+      <c r="B116" t="s">
+        <v>141</v>
+      </c>
+      <c r="C116" t="s">
+        <v>78</v>
+      </c>
+      <c r="D116" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117">
+        <v>115</v>
+      </c>
+      <c r="B117" t="s">
+        <v>140</v>
+      </c>
+      <c r="C117" t="s">
+        <v>78</v>
+      </c>
+      <c r="D117" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118">
+        <v>116</v>
+      </c>
+      <c r="B118" t="s">
+        <v>139</v>
+      </c>
+      <c r="C118" t="s">
+        <v>78</v>
+      </c>
+      <c r="D118" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119">
+        <v>117</v>
+      </c>
+      <c r="B119" t="s">
+        <v>138</v>
+      </c>
+      <c r="C119" t="s">
+        <v>78</v>
+      </c>
+      <c r="D119" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120">
+        <v>118</v>
+      </c>
+      <c r="B120" t="s">
+        <v>137</v>
+      </c>
+      <c r="C120" t="s">
+        <v>78</v>
+      </c>
+      <c r="D120" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121">
+        <v>119</v>
+      </c>
+      <c r="B121" t="s">
+        <v>136</v>
+      </c>
+      <c r="C121" t="s">
+        <v>78</v>
+      </c>
+      <c r="D121" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122">
+        <v>120</v>
+      </c>
+      <c r="B122" t="s">
+        <v>135</v>
+      </c>
+      <c r="C122" t="s">
+        <v>78</v>
+      </c>
+      <c r="D122" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123">
+        <v>121</v>
+      </c>
+      <c r="B123" t="s">
+        <v>134</v>
+      </c>
+      <c r="C123" t="s">
+        <v>78</v>
+      </c>
+      <c r="D123" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124">
+        <v>122</v>
+      </c>
+      <c r="B124" t="s">
+        <v>133</v>
+      </c>
+      <c r="C124" t="s">
+        <v>78</v>
+      </c>
+      <c r="D124" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125">
+        <v>123</v>
+      </c>
+      <c r="B125" t="s">
+        <v>132</v>
+      </c>
+      <c r="C125" t="s">
+        <v>78</v>
+      </c>
+      <c r="D125" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126">
+        <v>124</v>
+      </c>
+      <c r="B126" t="s">
+        <v>131</v>
+      </c>
+      <c r="C126" t="s">
+        <v>78</v>
+      </c>
+      <c r="D126" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127">
+        <v>125</v>
+      </c>
+      <c r="B127" t="s">
+        <v>130</v>
+      </c>
+      <c r="C127" t="s">
+        <v>78</v>
+      </c>
+      <c r="D127" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128">
+        <v>126</v>
+      </c>
+      <c r="B128" t="s">
+        <v>129</v>
+      </c>
+      <c r="C128" t="s">
+        <v>78</v>
+      </c>
+      <c r="D128" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129">
+        <v>127</v>
+      </c>
+      <c r="B129" t="s">
+        <v>128</v>
+      </c>
+      <c r="C129" t="s">
+        <v>78</v>
+      </c>
+      <c r="D129" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130">
+        <v>128</v>
+      </c>
+      <c r="B130" t="s">
+        <v>127</v>
+      </c>
+      <c r="C130" t="s">
+        <v>78</v>
+      </c>
+      <c r="D130" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131">
+        <v>129</v>
+      </c>
+      <c r="B131" t="s">
+        <v>126</v>
+      </c>
+      <c r="C131" t="s">
+        <v>78</v>
+      </c>
+      <c r="D131" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132">
+        <v>130</v>
+      </c>
+      <c r="B132" t="s">
+        <v>125</v>
+      </c>
+      <c r="C132" t="s">
+        <v>78</v>
+      </c>
+      <c r="D132" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133">
+        <v>131</v>
+      </c>
+      <c r="B133" t="s">
+        <v>124</v>
+      </c>
+      <c r="C133" t="s">
+        <v>78</v>
+      </c>
+      <c r="D133" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134">
+        <v>132</v>
+      </c>
+      <c r="B134" t="s">
+        <v>123</v>
+      </c>
+      <c r="C134" t="s">
+        <v>78</v>
+      </c>
+      <c r="D134" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135">
+        <v>133</v>
+      </c>
+      <c r="B135" t="s">
+        <v>122</v>
+      </c>
+      <c r="C135" t="s">
+        <v>78</v>
+      </c>
+      <c r="D135" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136">
+        <v>134</v>
+      </c>
+      <c r="B136" t="s">
+        <v>121</v>
+      </c>
+      <c r="C136" t="s">
+        <v>78</v>
+      </c>
+      <c r="D136" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137">
+        <v>135</v>
+      </c>
+      <c r="B137" t="s">
+        <v>120</v>
+      </c>
+      <c r="C137" t="s">
+        <v>78</v>
+      </c>
+      <c r="D137" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138">
+        <v>136</v>
+      </c>
+      <c r="B138" t="s">
+        <v>119</v>
+      </c>
+      <c r="C138" t="s">
+        <v>78</v>
+      </c>
+      <c r="D138" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139">
+        <v>137</v>
+      </c>
+      <c r="B139" t="s">
+        <v>118</v>
+      </c>
+      <c r="C139" t="s">
+        <v>78</v>
+      </c>
+      <c r="D139" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140">
+        <v>138</v>
+      </c>
+      <c r="B140" t="s">
+        <v>117</v>
+      </c>
+      <c r="C140" t="s">
+        <v>78</v>
+      </c>
+      <c r="D140" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141">
+        <v>139</v>
+      </c>
+      <c r="B141" t="s">
+        <v>116</v>
+      </c>
+      <c r="C141" t="s">
+        <v>78</v>
+      </c>
+      <c r="D141" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142">
+        <v>140</v>
+      </c>
+      <c r="B142" t="s">
+        <v>115</v>
+      </c>
+      <c r="C142" t="s">
+        <v>78</v>
+      </c>
+      <c r="D142" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143">
+        <v>141</v>
+      </c>
+      <c r="B143" t="s">
+        <v>114</v>
+      </c>
+      <c r="C143" t="s">
+        <v>78</v>
+      </c>
+      <c r="D143" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144">
+        <v>142</v>
+      </c>
+      <c r="B144" t="s">
+        <v>113</v>
+      </c>
+      <c r="C144" t="s">
+        <v>78</v>
+      </c>
+      <c r="D144" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145">
+        <v>143</v>
+      </c>
+      <c r="B145" t="s">
+        <v>112</v>
+      </c>
+      <c r="C145" t="s">
+        <v>78</v>
+      </c>
+      <c r="D145" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146">
+        <v>144</v>
+      </c>
+      <c r="B146" t="s">
+        <v>111</v>
+      </c>
+      <c r="C146" t="s">
+        <v>78</v>
+      </c>
+      <c r="D146" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147">
+        <v>145</v>
+      </c>
+      <c r="B147" t="s">
+        <v>110</v>
+      </c>
+      <c r="C147" t="s">
+        <v>78</v>
+      </c>
+      <c r="D147" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148">
+        <v>146</v>
+      </c>
+      <c r="B148" t="s">
+        <v>109</v>
+      </c>
+      <c r="C148" t="s">
+        <v>78</v>
+      </c>
+      <c r="D148" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149">
+        <v>147</v>
+      </c>
+      <c r="B149" t="s">
+        <v>108</v>
+      </c>
+      <c r="C149" t="s">
+        <v>78</v>
+      </c>
+      <c r="D149" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150">
+        <v>148</v>
+      </c>
+      <c r="B150" t="s">
+        <v>107</v>
+      </c>
+      <c r="C150" t="s">
+        <v>78</v>
+      </c>
+      <c r="D150" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151">
+        <v>149</v>
+      </c>
+      <c r="B151" t="s">
+        <v>106</v>
+      </c>
+      <c r="C151" t="s">
+        <v>78</v>
+      </c>
+      <c r="D151" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
configured to make first 1000 selections
</commit_message>
<xml_diff>
--- a/btsAccounts.xlsx
+++ b/btsAccounts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24526"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="0" windowWidth="25520" windowHeight="15620"/>
+    <workbookView xWindow="-240" yWindow="0" windowWidth="25520" windowHeight="15620"/>
   </bookViews>
   <sheets>
     <sheet name="Production" sheetId="1" r:id="rId1"/>
@@ -3460,8 +3460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A466" workbookViewId="0">
-      <selection activeCell="F501" sqref="F501"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>